<commit_message>
fix template image, tablecolumns, and image insert
</commit_message>
<xml_diff>
--- a/public/files/image_insert_template.xlsx
+++ b/public/files/image_insert_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SINAU\designyeuh-web\public\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wunonely\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BDC52E-C955-425F-841D-77719EFDAF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CD5FAE-0C98-4F5F-8BEC-0398792722CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{25E1AAA0-BA6B-40EB-BEE7-24E92C59A128}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +73,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,10 +109,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -132,8 +141,13 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,11 +466,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A576916-296E-4A45-9967-1526040FC49F}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -467,7 +481,8 @@
     <col min="5" max="5" width="18.6328125" style="7" customWidth="1"/>
     <col min="6" max="6" width="20.54296875" style="3" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="20.54296875" style="1" hidden="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="1" hidden="1"/>
+    <col min="8" max="8" width="20.54296875" style="1" hidden="1"/>
+    <col min="9" max="16384" width="8.7265625" style="1" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="51.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -488,6 +503,9 @@
       </c>
       <c r="F1" s="2"/>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D2" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>